<commit_message>
made FP template margins a bit more narrow
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_ФП.xlsx
+++ b/templates/ведомость_курсанты_ФП.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pronko\prj\Grader\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YUKI\3_Вирусы\Pronko_2\prj\Grader\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -441,6 +441,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -476,33 +503,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,7 +791,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="A5" sqref="A5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -806,76 +806,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
     </row>
     <row r="2" spans="1:20" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
@@ -900,179 +900,179 @@
       <c r="T4" s="21"/>
     </row>
     <row r="5" spans="1:20" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="37"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="46"/>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="37"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="46"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="39"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="48"/>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="29"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="38"/>
     </row>
     <row r="9" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="43" t="s">
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="43" t="s">
+      <c r="P9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="43" t="s">
+      <c r="Q9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="R9" s="43" t="s">
+      <c r="R9" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="S9" s="43" t="s">
+      <c r="S9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="T9" s="46" t="s">
+      <c r="T9" s="34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="41" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41" t="s">
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41" t="s">
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="47"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="35"/>
     </row>
     <row r="11" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="25" t="s">
         <v>36</v>
       </c>
@@ -1100,12 +1100,12 @@
       <c r="N11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="48"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="36"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
@@ -1330,28 +1330,28 @@
       <c r="T19" s="24"/>
     </row>
     <row r="20" spans="1:20" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
     </row>
     <row r="21" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
@@ -1585,6 +1585,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A8:T8"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A3:T3"/>
+    <mergeCell ref="A5:T5"/>
+    <mergeCell ref="A6:T6"/>
+    <mergeCell ref="A7:T7"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="I10:K10"/>
@@ -1601,16 +1608,9 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
-    <mergeCell ref="A8:T8"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A3:T3"/>
-    <mergeCell ref="A5:T5"/>
-    <mergeCell ref="A6:T6"/>
-    <mergeCell ref="A7:T7"/>
   </mergeCells>
-  <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="257" scale="68" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="257" scale="72" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>